<commit_message>
CIERRE 16 JUN 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #06  JUNIO 2022/BALANCE   HERRADURA  JUNIO      2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #06  JUNIO 2022/BALANCE   HERRADURA  JUNIO      2022.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16710" windowHeight="10305" firstSheet="10" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16710" windowHeight="10305" firstSheet="8" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="E N E R O    2 0 2 2         " sheetId="1" r:id="rId1"/>
@@ -384,7 +384,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="344">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -1407,6 +1407,15 @@
   </si>
   <si>
     <t>00141 D</t>
+  </si>
+  <si>
+    <t>CASERA-ARABE</t>
+  </si>
+  <si>
+    <t>NOMINA # 23</t>
+  </si>
+  <si>
+    <t>NOMIINA # 24</t>
   </si>
 </sst>
 </file>
@@ -2687,7 +2696,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="322">
+  <cellXfs count="317">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -3186,11 +3195,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="3" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="3" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="17" fillId="3" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="3" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -6198,23 +6202,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="283"/>
-      <c r="C1" s="285" t="s">
+      <c r="B1" s="278"/>
+      <c r="C1" s="280" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="286"/>
-      <c r="E1" s="286"/>
-      <c r="F1" s="286"/>
-      <c r="G1" s="286"/>
-      <c r="H1" s="286"/>
-      <c r="I1" s="286"/>
-      <c r="J1" s="286"/>
-      <c r="K1" s="286"/>
-      <c r="L1" s="286"/>
-      <c r="M1" s="286"/>
+      <c r="D1" s="281"/>
+      <c r="E1" s="281"/>
+      <c r="F1" s="281"/>
+      <c r="G1" s="281"/>
+      <c r="H1" s="281"/>
+      <c r="I1" s="281"/>
+      <c r="J1" s="281"/>
+      <c r="K1" s="281"/>
+      <c r="L1" s="281"/>
+      <c r="M1" s="281"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="284"/>
+      <c r="B2" s="279"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -6224,21 +6228,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="287" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="288"/>
+      <c r="B3" s="282" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="283"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="289" t="s">
+      <c r="H3" s="284" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="289"/>
+      <c r="I3" s="284"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="R3" s="294" t="s">
+      <c r="R3" s="289" t="s">
         <v>38</v>
       </c>
     </row>
@@ -6253,14 +6257,14 @@
       <c r="D4" s="18">
         <v>44563</v>
       </c>
-      <c r="E4" s="290" t="s">
+      <c r="E4" s="285" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="291"/>
-      <c r="H4" s="292" t="s">
+      <c r="F4" s="286"/>
+      <c r="H4" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="293"/>
+      <c r="I4" s="288"/>
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
       <c r="L4" s="21"/>
@@ -6270,11 +6274,11 @@
       <c r="N4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="301" t="s">
+      <c r="P4" s="296" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="302"/>
-      <c r="R4" s="295"/>
+      <c r="Q4" s="297"/>
+      <c r="R4" s="290"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
@@ -7775,11 +7779,11 @@
       <c r="J40" s="73"/>
       <c r="K40" s="89"/>
       <c r="L40" s="75"/>
-      <c r="M40" s="303">
+      <c r="M40" s="298">
         <f>SUM(M5:M39)</f>
         <v>1527030</v>
       </c>
-      <c r="N40" s="305">
+      <c r="N40" s="300">
         <f>SUM(N5:N39)</f>
         <v>50013</v>
       </c>
@@ -7805,8 +7809,8 @@
       <c r="J41" s="73"/>
       <c r="K41" s="76"/>
       <c r="L41" s="75"/>
-      <c r="M41" s="304"/>
-      <c r="N41" s="306"/>
+      <c r="M41" s="299"/>
+      <c r="N41" s="301"/>
       <c r="P41" s="34"/>
       <c r="Q41" s="9"/>
     </row>
@@ -8021,29 +8025,29 @@
       <c r="A53" s="117"/>
       <c r="B53" s="118"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="307" t="s">
+      <c r="H53" s="302" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="308"/>
+      <c r="I53" s="303"/>
       <c r="J53" s="119"/>
-      <c r="K53" s="309">
+      <c r="K53" s="304">
         <f>I51+L51</f>
         <v>50143.28</v>
       </c>
-      <c r="L53" s="310"/>
-      <c r="M53" s="311">
+      <c r="L53" s="305"/>
+      <c r="M53" s="306">
         <f>N40+M40</f>
         <v>1577043</v>
       </c>
-      <c r="N53" s="312"/>
+      <c r="N53" s="307"/>
       <c r="P53" s="34"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="313" t="s">
+      <c r="D54" s="308" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="313"/>
+      <c r="E54" s="308"/>
       <c r="F54" s="120">
         <f>F51-K53-C51</f>
         <v>1561421.72</v>
@@ -8054,22 +8058,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="314" t="s">
+      <c r="D55" s="309" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="314"/>
+      <c r="E55" s="309"/>
       <c r="F55" s="115">
         <v>-1419082.77</v>
       </c>
-      <c r="I55" s="315" t="s">
+      <c r="I55" s="310" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="316"/>
-      <c r="K55" s="317">
+      <c r="J55" s="311"/>
+      <c r="K55" s="312">
         <f>F57+F58+F59</f>
         <v>296963.46999999997</v>
       </c>
-      <c r="L55" s="318"/>
+      <c r="L55" s="313"/>
       <c r="P55" s="34"/>
       <c r="Q55" s="9"/>
     </row>
@@ -8100,11 +8104,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="130"/>
-      <c r="K57" s="319">
+      <c r="K57" s="314">
         <f>-C4</f>
         <v>-221059.7</v>
       </c>
-      <c r="L57" s="320"/>
+      <c r="L57" s="315"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="131" t="s">
@@ -8121,22 +8125,22 @@
       <c r="C59" s="133">
         <v>44591</v>
       </c>
-      <c r="D59" s="296" t="s">
+      <c r="D59" s="291" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="297"/>
+      <c r="E59" s="292"/>
       <c r="F59" s="134">
         <v>154314.51999999999</v>
       </c>
-      <c r="I59" s="298" t="s">
+      <c r="I59" s="293" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="299"/>
-      <c r="K59" s="300">
+      <c r="J59" s="294"/>
+      <c r="K59" s="295">
         <f>K55+K57</f>
         <v>75903.76999999996</v>
       </c>
-      <c r="L59" s="300"/>
+      <c r="L59" s="295"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="135"/>
@@ -9571,8 +9575,8 @@
   </sheetPr>
   <dimension ref="A1:U81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9591,27 +9595,27 @@
     <col min="14" max="14" width="16.140625" style="1" customWidth="1"/>
     <col min="16" max="16" width="18.42578125" customWidth="1"/>
     <col min="17" max="17" width="18.140625" style="244" customWidth="1"/>
-    <col min="18" max="18" width="14.85546875" style="3" customWidth="1"/>
+    <col min="18" max="18" width="14.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="283"/>
-      <c r="C1" s="285" t="s">
+      <c r="B1" s="278"/>
+      <c r="C1" s="280" t="s">
         <v>326</v>
       </c>
-      <c r="D1" s="286"/>
-      <c r="E1" s="286"/>
-      <c r="F1" s="286"/>
-      <c r="G1" s="286"/>
-      <c r="H1" s="286"/>
-      <c r="I1" s="286"/>
-      <c r="J1" s="286"/>
-      <c r="K1" s="286"/>
-      <c r="L1" s="286"/>
-      <c r="M1" s="286"/>
+      <c r="D1" s="281"/>
+      <c r="E1" s="281"/>
+      <c r="F1" s="281"/>
+      <c r="G1" s="281"/>
+      <c r="H1" s="281"/>
+      <c r="I1" s="281"/>
+      <c r="J1" s="281"/>
+      <c r="K1" s="281"/>
+      <c r="L1" s="281"/>
+      <c r="M1" s="281"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="284"/>
+      <c r="B2" s="279"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -9621,21 +9625,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="287" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="288"/>
+      <c r="B3" s="282" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="283"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="289" t="s">
+      <c r="H3" s="284" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="289"/>
+      <c r="I3" s="284"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="R3" s="294" t="s">
+      <c r="R3" s="289" t="s">
         <v>38</v>
       </c>
     </row>
@@ -9650,14 +9654,14 @@
       <c r="D4" s="18">
         <v>44710</v>
       </c>
-      <c r="E4" s="290" t="s">
+      <c r="E4" s="285" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="291"/>
-      <c r="H4" s="292" t="s">
+      <c r="F4" s="286"/>
+      <c r="H4" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="293"/>
+      <c r="I4" s="288"/>
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
       <c r="L4" s="21"/>
@@ -9667,11 +9671,11 @@
       <c r="N4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="301" t="s">
+      <c r="P4" s="296" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="302"/>
-      <c r="R4" s="295"/>
+      <c r="Q4" s="297"/>
+      <c r="R4" s="290"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
@@ -9680,30 +9684,37 @@
       <c r="B5" s="25">
         <v>44711</v>
       </c>
-      <c r="C5" s="26"/>
+      <c r="C5" s="26">
+        <v>0</v>
+      </c>
       <c r="D5" s="27"/>
       <c r="E5" s="28">
         <v>44711</v>
       </c>
-      <c r="F5" s="29"/>
+      <c r="F5" s="29">
+        <v>68569</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="30">
         <v>44711</v>
       </c>
-      <c r="I5" s="31"/>
+      <c r="I5" s="31">
+        <v>92</v>
+      </c>
       <c r="J5" s="7"/>
       <c r="K5" s="182"/>
       <c r="L5" s="9"/>
       <c r="M5" s="32">
-        <v>0</v>
+        <f>56619+11000</f>
+        <v>67619</v>
       </c>
       <c r="N5" s="33">
-        <v>0</v>
+        <v>858</v>
       </c>
       <c r="O5" s="2"/>
       <c r="P5" s="34">
         <f>N5+M5+L5+I5+C5</f>
-        <v>0</v>
+        <v>68569</v>
       </c>
       <c r="Q5" s="13">
         <f>P5-F5</f>
@@ -9716,58 +9727,75 @@
       <c r="B6" s="25">
         <v>44712</v>
       </c>
-      <c r="C6" s="26"/>
+      <c r="C6" s="26">
+        <v>0</v>
+      </c>
       <c r="D6" s="36"/>
       <c r="E6" s="28">
         <v>44712</v>
       </c>
-      <c r="F6" s="29"/>
+      <c r="F6" s="29">
+        <v>48343</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="30">
         <v>44712</v>
       </c>
-      <c r="I6" s="31"/>
+      <c r="I6" s="31">
+        <v>10</v>
+      </c>
       <c r="J6" s="38"/>
       <c r="K6" s="39"/>
       <c r="L6" s="40"/>
       <c r="M6" s="32">
-        <v>0</v>
+        <f>20000+40505</f>
+        <v>60505</v>
       </c>
       <c r="N6" s="33">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="34">
         <f t="shared" ref="P6:P34" si="0">N6+M6+L6+I6+C6</f>
-        <v>0</v>
+        <v>60715</v>
       </c>
       <c r="Q6" s="13">
-        <f t="shared" ref="Q6:Q40" si="1">P6-F6</f>
-        <v>0</v>
-      </c>
-      <c r="R6" s="8"/>
+        <v>0</v>
+      </c>
+      <c r="R6" s="184">
+        <v>12372</v>
+      </c>
     </row>
     <row r="7" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="24"/>
       <c r="B7" s="25">
         <v>44713</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="41"/>
+      <c r="C7" s="26">
+        <v>2830</v>
+      </c>
+      <c r="D7" s="41" t="s">
+        <v>341</v>
+      </c>
       <c r="E7" s="28">
         <v>44713</v>
       </c>
-      <c r="F7" s="29"/>
+      <c r="F7" s="29">
+        <v>45188</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="30">
         <v>44713</v>
       </c>
-      <c r="I7" s="31"/>
+      <c r="I7" s="31">
+        <v>87</v>
+      </c>
       <c r="J7" s="38"/>
       <c r="K7" s="42"/>
       <c r="L7" s="40"/>
       <c r="M7" s="32">
-        <v>0</v>
+        <f>27271+15000</f>
+        <v>42271</v>
       </c>
       <c r="N7" s="33">
         <v>0</v>
@@ -9775,10 +9803,10 @@
       <c r="O7" s="2"/>
       <c r="P7" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>45188</v>
       </c>
       <c r="Q7" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="Q7:Q40" si="1">P7-F7</f>
         <v>0</v>
       </c>
       <c r="R7" s="9"/>
@@ -9788,101 +9816,132 @@
       <c r="B8" s="25">
         <v>44714</v>
       </c>
-      <c r="C8" s="26"/>
+      <c r="C8" s="26">
+        <v>0</v>
+      </c>
       <c r="D8" s="41"/>
       <c r="E8" s="28">
         <v>44714</v>
       </c>
-      <c r="F8" s="29"/>
+      <c r="F8" s="29">
+        <v>70879</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="30">
         <v>44714</v>
       </c>
-      <c r="I8" s="31"/>
+      <c r="I8" s="31">
+        <v>30</v>
+      </c>
       <c r="J8" s="44"/>
       <c r="K8" s="45"/>
       <c r="L8" s="40"/>
       <c r="M8" s="32">
-        <v>0</v>
+        <f>41633+40000</f>
+        <v>81633</v>
       </c>
       <c r="N8" s="33">
-        <v>0</v>
+        <v>1977</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>83640</v>
       </c>
       <c r="Q8" s="13">
         <v>0</v>
       </c>
-      <c r="R8" s="9"/>
+      <c r="R8" s="184">
+        <v>12761</v>
+      </c>
     </row>
     <row r="9" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="24"/>
       <c r="B9" s="25">
         <v>44715</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="41"/>
+      <c r="C9" s="26">
+        <v>12937</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>49</v>
+      </c>
       <c r="E9" s="28">
         <v>44715</v>
       </c>
-      <c r="F9" s="29"/>
+      <c r="F9" s="29">
+        <v>99483</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="30">
         <v>44715</v>
       </c>
-      <c r="I9" s="31"/>
+      <c r="I9" s="31">
+        <v>123</v>
+      </c>
       <c r="J9" s="38"/>
       <c r="K9" s="46"/>
       <c r="L9" s="40"/>
       <c r="M9" s="32">
-        <v>0</v>
+        <f>61192+25000</f>
+        <v>86192</v>
       </c>
       <c r="N9" s="33">
-        <v>0</v>
+        <v>231</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="34">
-        <f>N9+M9+L9+I9+C9</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>99483</v>
       </c>
       <c r="Q9" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R9" s="8"/>
+      <c r="R9" s="9"/>
     </row>
     <row r="10" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="24"/>
       <c r="B10" s="25">
         <v>44716</v>
       </c>
-      <c r="C10" s="26"/>
+      <c r="C10" s="26">
+        <v>0</v>
+      </c>
       <c r="D10" s="36"/>
       <c r="E10" s="28">
         <v>44716</v>
       </c>
-      <c r="F10" s="29"/>
+      <c r="F10" s="29">
+        <v>104709</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="30">
         <v>44716</v>
       </c>
-      <c r="I10" s="31"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="48"/>
+      <c r="I10" s="31">
+        <v>99</v>
+      </c>
+      <c r="J10" s="38">
+        <v>44716</v>
+      </c>
+      <c r="K10" s="47" t="s">
+        <v>342</v>
+      </c>
+      <c r="L10" s="48">
+        <v>9483</v>
+      </c>
       <c r="M10" s="32">
-        <v>0</v>
+        <f>35000+49514+675</f>
+        <v>85189</v>
       </c>
       <c r="N10" s="33">
-        <v>0</v>
+        <v>9938</v>
       </c>
       <c r="O10" s="2"/>
       <c r="P10" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>104709</v>
       </c>
       <c r="Q10" s="13">
         <f t="shared" si="1"/>
@@ -9898,36 +9957,43 @@
       <c r="B11" s="25">
         <v>44717</v>
       </c>
-      <c r="C11" s="26"/>
+      <c r="C11" s="26">
+        <v>0</v>
+      </c>
       <c r="D11" s="36"/>
       <c r="E11" s="28">
         <v>44717</v>
       </c>
-      <c r="F11" s="29"/>
+      <c r="F11" s="29">
+        <v>122844</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="30">
         <v>44717</v>
       </c>
-      <c r="I11" s="31"/>
+      <c r="I11" s="31">
+        <v>0</v>
+      </c>
       <c r="J11" s="44"/>
       <c r="K11" s="49"/>
       <c r="L11" s="40"/>
       <c r="M11" s="32">
-        <v>0</v>
+        <f>32526+90000</f>
+        <v>122526</v>
       </c>
       <c r="N11" s="33">
-        <v>0</v>
+        <v>318</v>
       </c>
       <c r="O11" s="2"/>
       <c r="P11" s="34">
         <f>N11+M11+L11+I11+C11</f>
-        <v>0</v>
+        <v>122844</v>
       </c>
       <c r="Q11" s="13">
-        <f>P11-F11</f>
-        <v>0</v>
-      </c>
-      <c r="R11" s="8" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R11" s="9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -9936,22 +10002,31 @@
       <c r="B12" s="25">
         <v>44718</v>
       </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="36"/>
+      <c r="C12" s="26">
+        <v>3600</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>47</v>
+      </c>
       <c r="E12" s="28">
         <v>44718</v>
       </c>
-      <c r="F12" s="29"/>
+      <c r="F12" s="29">
+        <v>87892</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="30">
         <v>44718</v>
       </c>
-      <c r="I12" s="31"/>
+      <c r="I12" s="31">
+        <v>65</v>
+      </c>
       <c r="J12" s="38"/>
       <c r="K12" s="50"/>
       <c r="L12" s="40"/>
       <c r="M12" s="32">
-        <v>0</v>
+        <f>36227+48000</f>
+        <v>84227</v>
       </c>
       <c r="N12" s="33">
         <v>0</v>
@@ -9959,43 +10034,52 @@
       <c r="O12" s="2"/>
       <c r="P12" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>87892</v>
       </c>
       <c r="Q12" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R12" s="8"/>
+      <c r="R12" s="9"/>
     </row>
     <row r="13" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="24"/>
       <c r="B13" s="25">
         <v>44719</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="41"/>
+      <c r="C13" s="26">
+        <v>800</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>133</v>
+      </c>
       <c r="E13" s="28">
         <v>44719</v>
       </c>
-      <c r="F13" s="29"/>
+      <c r="F13" s="29">
+        <v>72961</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="30">
         <v>44719</v>
       </c>
-      <c r="I13" s="31"/>
+      <c r="I13" s="31">
+        <v>127</v>
+      </c>
       <c r="J13" s="38"/>
       <c r="K13" s="39"/>
       <c r="L13" s="40"/>
       <c r="M13" s="32">
-        <v>0</v>
+        <f>33794+20000</f>
+        <v>53794</v>
       </c>
       <c r="N13" s="33">
-        <v>0</v>
+        <v>18240</v>
       </c>
       <c r="O13" s="2"/>
       <c r="P13" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>72961</v>
       </c>
       <c r="Q13" s="13">
         <f t="shared" si="1"/>
@@ -10008,30 +10092,37 @@
       <c r="B14" s="25">
         <v>44720</v>
       </c>
-      <c r="C14" s="26"/>
+      <c r="C14" s="26">
+        <v>0</v>
+      </c>
       <c r="D14" s="51"/>
       <c r="E14" s="28">
         <v>44720</v>
       </c>
-      <c r="F14" s="29"/>
+      <c r="F14" s="29">
+        <v>43378</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="30">
         <v>44720</v>
       </c>
-      <c r="I14" s="31"/>
+      <c r="I14" s="31">
+        <v>60</v>
+      </c>
       <c r="J14" s="38"/>
       <c r="K14" s="45"/>
       <c r="L14" s="40"/>
       <c r="M14" s="32">
-        <v>0</v>
+        <f>28218+15000</f>
+        <v>43218</v>
       </c>
       <c r="N14" s="33">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O14" s="2"/>
       <c r="P14" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>43378</v>
       </c>
       <c r="Q14" s="13">
         <f t="shared" si="1"/>
@@ -10044,70 +10135,86 @@
       <c r="B15" s="25">
         <v>44721</v>
       </c>
-      <c r="C15" s="26"/>
+      <c r="C15" s="26">
+        <v>0</v>
+      </c>
       <c r="D15" s="51"/>
       <c r="E15" s="28">
         <v>44721</v>
       </c>
-      <c r="F15" s="29"/>
+      <c r="F15" s="29">
+        <v>74534</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="30">
         <v>44721</v>
       </c>
-      <c r="I15" s="31"/>
+      <c r="I15" s="31">
+        <v>31</v>
+      </c>
       <c r="J15" s="38"/>
       <c r="K15" s="45"/>
       <c r="L15" s="40"/>
       <c r="M15" s="32">
-        <v>0</v>
+        <f>15000+59275</f>
+        <v>74275</v>
       </c>
       <c r="N15" s="33">
-        <v>0</v>
+        <v>228</v>
       </c>
       <c r="P15" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>74534</v>
       </c>
       <c r="Q15" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R15" s="8"/>
+      <c r="R15" s="9"/>
     </row>
     <row r="16" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="24"/>
       <c r="B16" s="25">
         <v>44722</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="36"/>
+      <c r="C16" s="26">
+        <v>23100</v>
+      </c>
+      <c r="D16" s="36" t="s">
+        <v>49</v>
+      </c>
       <c r="E16" s="28">
         <v>44722</v>
       </c>
-      <c r="F16" s="29"/>
+      <c r="F16" s="29">
+        <v>137137</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="30">
         <v>44722</v>
       </c>
-      <c r="I16" s="31"/>
+      <c r="I16" s="31">
+        <v>208</v>
+      </c>
       <c r="J16" s="38"/>
       <c r="K16" s="45"/>
       <c r="L16" s="9"/>
       <c r="M16" s="32">
-        <v>0</v>
+        <f>83015+30000</f>
+        <v>113015</v>
       </c>
       <c r="N16" s="33">
-        <v>0</v>
+        <v>814</v>
       </c>
       <c r="P16" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>137137</v>
       </c>
       <c r="Q16" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R16" s="8" t="s">
+      <c r="R16" s="9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -10116,20 +10223,34 @@
       <c r="B17" s="25">
         <v>44723</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="41"/>
+      <c r="C17" s="26">
+        <v>3430</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>47</v>
+      </c>
       <c r="E17" s="28">
         <v>44723</v>
       </c>
-      <c r="F17" s="29"/>
+      <c r="F17" s="29">
+        <v>91767</v>
+      </c>
       <c r="G17" s="2"/>
       <c r="H17" s="30">
         <v>44723</v>
       </c>
-      <c r="I17" s="31"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="52"/>
-      <c r="L17" s="48"/>
+      <c r="I17" s="31">
+        <v>60</v>
+      </c>
+      <c r="J17" s="38">
+        <v>44723</v>
+      </c>
+      <c r="K17" s="52" t="s">
+        <v>343</v>
+      </c>
+      <c r="L17" s="48">
+        <v>9500</v>
+      </c>
       <c r="M17" s="32">
         <v>0</v>
       </c>
@@ -10138,20 +10259,22 @@
       </c>
       <c r="P17" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12990</v>
       </c>
       <c r="Q17" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R17" s="8"/>
+        <v>-78777</v>
+      </c>
+      <c r="R17" s="9"/>
     </row>
     <row r="18" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="24"/>
       <c r="B18" s="25">
         <v>44724</v>
       </c>
-      <c r="C18" s="26"/>
+      <c r="C18" s="26">
+        <v>0</v>
+      </c>
       <c r="D18" s="36"/>
       <c r="E18" s="28">
         <v>44724</v>
@@ -10179,14 +10302,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R18" s="8"/>
+      <c r="R18" s="9"/>
     </row>
     <row r="19" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="24"/>
       <c r="B19" s="25">
         <v>44725</v>
       </c>
-      <c r="C19" s="26"/>
+      <c r="C19" s="26">
+        <v>0</v>
+      </c>
       <c r="D19" s="36"/>
       <c r="E19" s="28">
         <v>44725</v>
@@ -10215,14 +10340,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R19" s="8"/>
+      <c r="R19" s="9"/>
     </row>
     <row r="20" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="24"/>
       <c r="B20" s="25">
         <v>44726</v>
       </c>
-      <c r="C20" s="26"/>
+      <c r="C20" s="26">
+        <v>0</v>
+      </c>
       <c r="D20" s="36"/>
       <c r="E20" s="28">
         <v>44726</v>
@@ -10250,14 +10377,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R20" s="8"/>
+      <c r="R20" s="9"/>
     </row>
     <row r="21" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="24"/>
       <c r="B21" s="25">
         <v>44727</v>
       </c>
-      <c r="C21" s="26"/>
+      <c r="C21" s="26">
+        <v>0</v>
+      </c>
       <c r="D21" s="36"/>
       <c r="E21" s="28">
         <v>44727</v>
@@ -10285,14 +10414,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R21" s="8"/>
+      <c r="R21" s="9"/>
     </row>
     <row r="22" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="24"/>
       <c r="B22" s="25">
         <v>44728</v>
       </c>
-      <c r="C22" s="26"/>
+      <c r="C22" s="26">
+        <v>0</v>
+      </c>
       <c r="D22" s="36"/>
       <c r="E22" s="28">
         <v>44728</v>
@@ -10320,14 +10451,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R22" s="8"/>
+      <c r="R22" s="9"/>
     </row>
     <row r="23" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="24"/>
       <c r="B23" s="25">
         <v>44729</v>
       </c>
-      <c r="C23" s="26"/>
+      <c r="C23" s="26">
+        <v>0</v>
+      </c>
       <c r="D23" s="36"/>
       <c r="E23" s="28">
         <v>44729</v>
@@ -10355,14 +10488,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R23" s="8"/>
+      <c r="R23" s="9"/>
     </row>
     <row r="24" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="24"/>
       <c r="B24" s="25">
         <v>44730</v>
       </c>
-      <c r="C24" s="26"/>
+      <c r="C24" s="26">
+        <v>0</v>
+      </c>
       <c r="D24" s="41"/>
       <c r="E24" s="28">
         <v>44730</v>
@@ -10390,14 +10525,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R24" s="8"/>
+      <c r="R24" s="9"/>
     </row>
     <row r="25" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="24"/>
       <c r="B25" s="25">
         <v>44731</v>
       </c>
-      <c r="C25" s="26"/>
+      <c r="C25" s="26">
+        <v>0</v>
+      </c>
       <c r="D25" s="36"/>
       <c r="E25" s="28">
         <v>44731</v>
@@ -10428,14 +10565,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R25" s="8"/>
+      <c r="R25" s="9"/>
     </row>
     <row r="26" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="24"/>
       <c r="B26" s="25">
         <v>44732</v>
       </c>
-      <c r="C26" s="26"/>
+      <c r="C26" s="26">
+        <v>0</v>
+      </c>
       <c r="D26" s="36"/>
       <c r="E26" s="28">
         <v>44732</v>
@@ -10470,7 +10609,9 @@
       <c r="B27" s="25">
         <v>44733</v>
       </c>
-      <c r="C27" s="26"/>
+      <c r="C27" s="26">
+        <v>0</v>
+      </c>
       <c r="D27" s="41"/>
       <c r="E27" s="28">
         <v>44733</v>
@@ -10498,14 +10639,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R27" s="8"/>
+      <c r="R27" s="9"/>
     </row>
     <row r="28" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="24"/>
       <c r="B28" s="25">
         <v>44734</v>
       </c>
-      <c r="C28" s="26"/>
+      <c r="C28" s="26">
+        <v>0</v>
+      </c>
       <c r="D28" s="41"/>
       <c r="E28" s="28">
         <v>44734</v>
@@ -10533,14 +10676,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R28" s="8"/>
+      <c r="R28" s="9"/>
     </row>
     <row r="29" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="24"/>
       <c r="B29" s="25">
         <v>44735</v>
       </c>
-      <c r="C29" s="26"/>
+      <c r="C29" s="26">
+        <v>0</v>
+      </c>
       <c r="D29" s="71"/>
       <c r="E29" s="28">
         <v>44735</v>
@@ -10568,14 +10713,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R29" s="8"/>
+      <c r="R29" s="9"/>
     </row>
     <row r="30" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="24"/>
       <c r="B30" s="25">
         <v>44736</v>
       </c>
-      <c r="C30" s="26"/>
+      <c r="C30" s="26">
+        <v>0</v>
+      </c>
       <c r="D30" s="71"/>
       <c r="E30" s="28">
         <v>44736</v>
@@ -10603,14 +10750,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R30" s="8"/>
+      <c r="R30" s="9"/>
     </row>
     <row r="31" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="24"/>
       <c r="B31" s="25">
         <v>44737</v>
       </c>
-      <c r="C31" s="26"/>
+      <c r="C31" s="26">
+        <v>0</v>
+      </c>
       <c r="D31" s="83"/>
       <c r="E31" s="28">
         <v>44737</v>
@@ -10638,14 +10787,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R31" s="8"/>
+      <c r="R31" s="9"/>
     </row>
     <row r="32" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="24"/>
       <c r="B32" s="25">
         <v>44738</v>
       </c>
-      <c r="C32" s="26"/>
+      <c r="C32" s="26">
+        <v>0</v>
+      </c>
       <c r="D32" s="78"/>
       <c r="E32" s="28">
         <v>44738</v>
@@ -10673,7 +10824,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R32" s="8" t="s">
+      <c r="R32" s="9" t="s">
         <v>131</v>
       </c>
     </row>
@@ -10682,7 +10833,9 @@
       <c r="B33" s="25">
         <v>44739</v>
       </c>
-      <c r="C33" s="26"/>
+      <c r="C33" s="26">
+        <v>0</v>
+      </c>
       <c r="D33" s="79"/>
       <c r="E33" s="28">
         <v>44739</v>
@@ -10706,18 +10859,20 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q33" s="61">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R33" s="8"/>
+      <c r="Q33" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R33" s="9"/>
     </row>
     <row r="34" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="24"/>
       <c r="B34" s="25">
         <v>44740</v>
       </c>
-      <c r="C34" s="26"/>
+      <c r="C34" s="26">
+        <v>0</v>
+      </c>
       <c r="D34" s="78"/>
       <c r="E34" s="28">
         <v>44740</v>
@@ -10745,7 +10900,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R34" s="8" t="s">
+      <c r="R34" s="9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -10754,7 +10909,9 @@
       <c r="B35" s="25">
         <v>44741</v>
       </c>
-      <c r="C35" s="26"/>
+      <c r="C35" s="26">
+        <v>0</v>
+      </c>
       <c r="D35" s="83"/>
       <c r="E35" s="28">
         <v>44741</v>
@@ -10781,14 +10938,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R35" s="8"/>
+      <c r="R35" s="9"/>
     </row>
     <row r="36" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="24"/>
       <c r="B36" s="25">
         <v>44742</v>
       </c>
-      <c r="C36" s="26"/>
+      <c r="C36" s="26">
+        <v>0</v>
+      </c>
       <c r="D36" s="84"/>
       <c r="E36" s="28">
         <v>44742</v>
@@ -10815,14 +10974,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R36" s="8"/>
+      <c r="R36" s="9"/>
     </row>
     <row r="37" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="24"/>
       <c r="B37" s="25">
         <v>44743</v>
       </c>
-      <c r="C37" s="26"/>
+      <c r="C37" s="26">
+        <v>0</v>
+      </c>
       <c r="D37" s="78"/>
       <c r="E37" s="28">
         <v>44743</v>
@@ -10855,7 +11016,9 @@
       <c r="B38" s="25">
         <v>44744</v>
       </c>
-      <c r="C38" s="26"/>
+      <c r="C38" s="26">
+        <v>0</v>
+      </c>
       <c r="D38" s="79"/>
       <c r="E38" s="28">
         <v>44744</v>
@@ -10878,7 +11041,7 @@
       <c r="P38" s="34">
         <v>0</v>
       </c>
-      <c r="Q38" s="61">
+      <c r="Q38" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -10888,7 +11051,9 @@
       <c r="B39" s="25">
         <v>44745</v>
       </c>
-      <c r="C39" s="26"/>
+      <c r="C39" s="26">
+        <v>0</v>
+      </c>
       <c r="D39" s="79"/>
       <c r="E39" s="28">
         <v>44745</v>
@@ -10900,7 +11065,7 @@
       </c>
       <c r="I39" s="31"/>
       <c r="J39" s="73"/>
-      <c r="K39" s="282"/>
+      <c r="K39" s="277"/>
       <c r="L39" s="75"/>
       <c r="M39" s="32">
         <v>0</v>
@@ -10929,21 +11094,21 @@
       <c r="J40" s="73"/>
       <c r="K40" s="76"/>
       <c r="L40" s="75"/>
-      <c r="M40" s="303">
+      <c r="M40" s="298">
         <f>SUM(M5:M39)</f>
-        <v>0</v>
-      </c>
-      <c r="N40" s="305">
+        <v>914464</v>
+      </c>
+      <c r="N40" s="300">
         <f>SUM(N5:N39)</f>
-        <v>0</v>
+        <v>32904</v>
       </c>
       <c r="P40" s="34">
         <f>SUM(P5:P39)</f>
-        <v>0</v>
+        <v>1014040</v>
       </c>
       <c r="Q40" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1014040</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -10959,8 +11124,8 @@
       <c r="J41" s="73"/>
       <c r="K41" s="245"/>
       <c r="L41" s="75"/>
-      <c r="M41" s="304"/>
-      <c r="N41" s="306"/>
+      <c r="M41" s="299"/>
+      <c r="N41" s="301"/>
       <c r="P41" s="34"/>
       <c r="Q41" s="9"/>
     </row>
@@ -11133,7 +11298,7 @@
       </c>
       <c r="C51" s="106">
         <f>SUM(C5:C50)</f>
-        <v>0</v>
+        <v>46697</v>
       </c>
       <c r="D51" s="107"/>
       <c r="E51" s="108" t="s">
@@ -11141,7 +11306,7 @@
       </c>
       <c r="F51" s="109">
         <f>SUM(F5:F50)</f>
-        <v>0</v>
+        <v>1067684</v>
       </c>
       <c r="G51" s="107"/>
       <c r="H51" s="110" t="s">
@@ -11149,7 +11314,7 @@
       </c>
       <c r="I51" s="111">
         <f>SUM(I5:I50)</f>
-        <v>0</v>
+        <v>992</v>
       </c>
       <c r="J51" s="112"/>
       <c r="K51" s="113" t="s">
@@ -11157,7 +11322,7 @@
       </c>
       <c r="L51" s="114">
         <f>SUM(L5:L50)</f>
-        <v>0</v>
+        <v>18983</v>
       </c>
       <c r="M51" s="115"/>
       <c r="N51" s="115"/>
@@ -11175,32 +11340,32 @@
       <c r="A53" s="117"/>
       <c r="B53" s="118"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="307" t="s">
+      <c r="H53" s="302" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="308"/>
+      <c r="I53" s="303"/>
       <c r="J53" s="119"/>
-      <c r="K53" s="309">
+      <c r="K53" s="304">
         <f>I51+L51</f>
-        <v>0</v>
-      </c>
-      <c r="L53" s="310"/>
-      <c r="M53" s="311">
+        <v>19975</v>
+      </c>
+      <c r="L53" s="305"/>
+      <c r="M53" s="306">
         <f>N40+M40</f>
-        <v>0</v>
-      </c>
-      <c r="N53" s="312"/>
+        <v>947368</v>
+      </c>
+      <c r="N53" s="307"/>
       <c r="P53" s="34"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="313" t="s">
+      <c r="D54" s="308" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="313"/>
+      <c r="E54" s="308"/>
       <c r="F54" s="120">
         <f>F51-K53-C51</f>
-        <v>0</v>
+        <v>1001012</v>
       </c>
       <c r="I54" s="121"/>
       <c r="J54" s="122"/>
@@ -11208,22 +11373,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="314" t="s">
+      <c r="D55" s="309" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="314"/>
+      <c r="E55" s="309"/>
       <c r="F55" s="115">
         <v>0</v>
       </c>
-      <c r="I55" s="315" t="s">
+      <c r="I55" s="310" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="316"/>
-      <c r="K55" s="317">
+      <c r="J55" s="311"/>
+      <c r="K55" s="312">
         <f>F57+F58+F59</f>
-        <v>0</v>
-      </c>
-      <c r="L55" s="318"/>
+        <v>1001012</v>
+      </c>
+      <c r="L55" s="313"/>
       <c r="P55" s="34"/>
       <c r="Q55" s="9"/>
     </row>
@@ -11247,18 +11412,18 @@
       </c>
       <c r="F57" s="115">
         <f>SUM(F54:F56)</f>
-        <v>0</v>
+        <v>1001012</v>
       </c>
       <c r="H57" s="24"/>
       <c r="I57" s="129" t="s">
         <v>17</v>
       </c>
       <c r="J57" s="130"/>
-      <c r="K57" s="319">
+      <c r="K57" s="314">
         <f>-C4</f>
         <v>-149938.81</v>
       </c>
-      <c r="L57" s="320"/>
+      <c r="L57" s="315"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="131" t="s">
@@ -11273,22 +11438,22 @@
     </row>
     <row r="59" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C59" s="133"/>
-      <c r="D59" s="296" t="s">
+      <c r="D59" s="291" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="297"/>
+      <c r="E59" s="292"/>
       <c r="F59" s="134">
         <v>0</v>
       </c>
-      <c r="I59" s="298" t="s">
+      <c r="I59" s="293" t="s">
         <v>325</v>
       </c>
-      <c r="J59" s="299"/>
-      <c r="K59" s="300">
+      <c r="J59" s="294"/>
+      <c r="K59" s="295">
         <f>K55+K57</f>
-        <v>-149938.81</v>
-      </c>
-      <c r="L59" s="300"/>
+        <v>851073.19</v>
+      </c>
+      <c r="L59" s="295"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="135"/>
@@ -11442,20 +11607,20 @@
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="I59:J59"/>
     <mergeCell ref="K59:L59"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="M40:M41"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="D54:E54"/>
     <mergeCell ref="N40:N41"/>
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="M53:N53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="P4:Q4"/>
   </mergeCells>
   <pageMargins left="0.38" right="0.17" top="0.4" bottom="0.34" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -14425,23 +14590,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="283"/>
-      <c r="C1" s="285" t="s">
+      <c r="B1" s="278"/>
+      <c r="C1" s="280" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="286"/>
-      <c r="E1" s="286"/>
-      <c r="F1" s="286"/>
-      <c r="G1" s="286"/>
-      <c r="H1" s="286"/>
-      <c r="I1" s="286"/>
-      <c r="J1" s="286"/>
-      <c r="K1" s="286"/>
-      <c r="L1" s="286"/>
-      <c r="M1" s="286"/>
+      <c r="D1" s="281"/>
+      <c r="E1" s="281"/>
+      <c r="F1" s="281"/>
+      <c r="G1" s="281"/>
+      <c r="H1" s="281"/>
+      <c r="I1" s="281"/>
+      <c r="J1" s="281"/>
+      <c r="K1" s="281"/>
+      <c r="L1" s="281"/>
+      <c r="M1" s="281"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="284"/>
+      <c r="B2" s="279"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -14451,21 +14616,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="287" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="288"/>
+      <c r="B3" s="282" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="283"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="289" t="s">
+      <c r="H3" s="284" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="289"/>
+      <c r="I3" s="284"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="R3" s="294" t="s">
+      <c r="R3" s="289" t="s">
         <v>38</v>
       </c>
     </row>
@@ -14480,14 +14645,14 @@
       <c r="D4" s="18">
         <v>44591</v>
       </c>
-      <c r="E4" s="290" t="s">
+      <c r="E4" s="285" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="291"/>
-      <c r="H4" s="292" t="s">
+      <c r="F4" s="286"/>
+      <c r="H4" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="293"/>
+      <c r="I4" s="288"/>
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
       <c r="L4" s="21"/>
@@ -14497,11 +14662,11 @@
       <c r="N4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="301" t="s">
+      <c r="P4" s="296" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="302"/>
-      <c r="R4" s="295"/>
+      <c r="Q4" s="297"/>
+      <c r="R4" s="290"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
@@ -15985,11 +16150,11 @@
       <c r="J40" s="73"/>
       <c r="K40" s="89"/>
       <c r="L40" s="80"/>
-      <c r="M40" s="321">
+      <c r="M40" s="316">
         <f>SUM(M5:M39)</f>
         <v>1636108</v>
       </c>
-      <c r="N40" s="305">
+      <c r="N40" s="300">
         <f>SUM(N5:N39)</f>
         <v>55675</v>
       </c>
@@ -16015,8 +16180,8 @@
       <c r="J41" s="73"/>
       <c r="K41" s="76"/>
       <c r="L41" s="75"/>
-      <c r="M41" s="304"/>
-      <c r="N41" s="306"/>
+      <c r="M41" s="299"/>
+      <c r="N41" s="301"/>
       <c r="P41" s="34"/>
       <c r="Q41" s="9"/>
     </row>
@@ -16231,29 +16396,29 @@
       <c r="A53" s="117"/>
       <c r="B53" s="118"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="307" t="s">
+      <c r="H53" s="302" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="308"/>
+      <c r="I53" s="303"/>
       <c r="J53" s="119"/>
-      <c r="K53" s="309">
+      <c r="K53" s="304">
         <f>I51+L51</f>
         <v>45634.280000000006</v>
       </c>
-      <c r="L53" s="310"/>
-      <c r="M53" s="311">
+      <c r="L53" s="305"/>
+      <c r="M53" s="306">
         <f>N40+M40</f>
         <v>1691783</v>
       </c>
-      <c r="N53" s="312"/>
+      <c r="N53" s="307"/>
       <c r="P53" s="34"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="313" t="s">
+      <c r="D54" s="308" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="313"/>
+      <c r="E54" s="308"/>
       <c r="F54" s="120">
         <f>F51-K53-C51</f>
         <v>1686442.72</v>
@@ -16264,22 +16429,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="314" t="s">
+      <c r="D55" s="309" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="314"/>
+      <c r="E55" s="309"/>
       <c r="F55" s="115">
         <v>-1631962.77</v>
       </c>
-      <c r="I55" s="315" t="s">
+      <c r="I55" s="310" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="316"/>
-      <c r="K55" s="317">
+      <c r="J55" s="311"/>
+      <c r="K55" s="312">
         <f>F57+F58+F59</f>
         <v>238822.13999999996</v>
       </c>
-      <c r="L55" s="318"/>
+      <c r="L55" s="313"/>
       <c r="P55" s="34"/>
       <c r="Q55" s="9"/>
     </row>
@@ -16310,11 +16475,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="130"/>
-      <c r="K57" s="319">
+      <c r="K57" s="314">
         <f>-C4</f>
         <v>-154314.51999999999</v>
       </c>
-      <c r="L57" s="320"/>
+      <c r="L57" s="315"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="131" t="s">
@@ -16331,22 +16496,22 @@
       <c r="C59" s="133">
         <v>44619</v>
       </c>
-      <c r="D59" s="296" t="s">
+      <c r="D59" s="291" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="297"/>
+      <c r="E59" s="292"/>
       <c r="F59" s="134">
         <v>184342.19</v>
       </c>
-      <c r="I59" s="298" t="s">
+      <c r="I59" s="293" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="299"/>
-      <c r="K59" s="300">
+      <c r="J59" s="294"/>
+      <c r="K59" s="295">
         <f>K55+K57</f>
         <v>84507.619999999966</v>
       </c>
-      <c r="L59" s="300"/>
+      <c r="L59" s="295"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="135"/>
@@ -17815,23 +17980,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="283"/>
-      <c r="C1" s="285" t="s">
+      <c r="B1" s="278"/>
+      <c r="C1" s="280" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="286"/>
-      <c r="E1" s="286"/>
-      <c r="F1" s="286"/>
-      <c r="G1" s="286"/>
-      <c r="H1" s="286"/>
-      <c r="I1" s="286"/>
-      <c r="J1" s="286"/>
-      <c r="K1" s="286"/>
-      <c r="L1" s="286"/>
-      <c r="M1" s="286"/>
+      <c r="D1" s="281"/>
+      <c r="E1" s="281"/>
+      <c r="F1" s="281"/>
+      <c r="G1" s="281"/>
+      <c r="H1" s="281"/>
+      <c r="I1" s="281"/>
+      <c r="J1" s="281"/>
+      <c r="K1" s="281"/>
+      <c r="L1" s="281"/>
+      <c r="M1" s="281"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="284"/>
+      <c r="B2" s="279"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -17841,21 +18006,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="287" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="288"/>
+      <c r="B3" s="282" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="283"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="289" t="s">
+      <c r="H3" s="284" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="289"/>
+      <c r="I3" s="284"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="R3" s="294" t="s">
+      <c r="R3" s="289" t="s">
         <v>38</v>
       </c>
     </row>
@@ -17870,14 +18035,14 @@
       <c r="D4" s="18">
         <v>44619</v>
       </c>
-      <c r="E4" s="290" t="s">
+      <c r="E4" s="285" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="291"/>
-      <c r="H4" s="292" t="s">
+      <c r="F4" s="286"/>
+      <c r="H4" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="293"/>
+      <c r="I4" s="288"/>
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
       <c r="L4" s="21"/>
@@ -17887,11 +18052,11 @@
       <c r="N4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="301" t="s">
+      <c r="P4" s="296" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="302"/>
-      <c r="R4" s="295"/>
+      <c r="Q4" s="297"/>
+      <c r="R4" s="290"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
@@ -19188,10 +19353,10 @@
       <c r="J34" s="73">
         <v>44627</v>
       </c>
-      <c r="K34" s="277" t="s">
+      <c r="K34" s="272" t="s">
         <v>321</v>
       </c>
-      <c r="L34" s="280">
+      <c r="L34" s="275">
         <v>1195.68</v>
       </c>
       <c r="M34" s="32">
@@ -19258,7 +19423,7 @@
       <c r="J36" s="73">
         <v>44645</v>
       </c>
-      <c r="K36" s="279" t="s">
+      <c r="K36" s="274" t="s">
         <v>318</v>
       </c>
       <c r="L36" s="80">
@@ -19293,7 +19458,7 @@
       <c r="J37" s="73">
         <v>44649</v>
       </c>
-      <c r="K37" s="278" t="s">
+      <c r="K37" s="273" t="s">
         <v>319</v>
       </c>
       <c r="L37" s="80">
@@ -19327,7 +19492,7 @@
       <c r="J38" s="73">
         <v>44649</v>
       </c>
-      <c r="K38" s="281" t="s">
+      <c r="K38" s="276" t="s">
         <v>190</v>
       </c>
       <c r="L38" s="80">
@@ -19389,11 +19554,11 @@
       <c r="J40" s="73"/>
       <c r="K40" s="89"/>
       <c r="L40" s="75"/>
-      <c r="M40" s="303">
+      <c r="M40" s="298">
         <f>SUM(M5:M39)</f>
         <v>1793435</v>
       </c>
-      <c r="N40" s="305">
+      <c r="N40" s="300">
         <f>SUM(N5:N39)</f>
         <v>63995</v>
       </c>
@@ -19419,8 +19584,8 @@
       <c r="J41" s="73"/>
       <c r="K41" s="245"/>
       <c r="L41" s="75"/>
-      <c r="M41" s="304"/>
-      <c r="N41" s="306"/>
+      <c r="M41" s="299"/>
+      <c r="N41" s="301"/>
       <c r="P41" s="34"/>
       <c r="Q41" s="9"/>
     </row>
@@ -19563,29 +19728,29 @@
       <c r="A49" s="117"/>
       <c r="B49" s="118"/>
       <c r="C49" s="1"/>
-      <c r="H49" s="307" t="s">
+      <c r="H49" s="302" t="s">
         <v>12</v>
       </c>
-      <c r="I49" s="308"/>
+      <c r="I49" s="303"/>
       <c r="J49" s="119"/>
-      <c r="K49" s="309">
+      <c r="K49" s="304">
         <f>I47+L47</f>
         <v>90434.03</v>
       </c>
-      <c r="L49" s="310"/>
-      <c r="M49" s="311">
+      <c r="L49" s="305"/>
+      <c r="M49" s="306">
         <f>N40+M40</f>
         <v>1857430</v>
       </c>
-      <c r="N49" s="312"/>
+      <c r="N49" s="307"/>
       <c r="P49" s="34"/>
       <c r="Q49" s="9"/>
     </row>
     <row r="50" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D50" s="313" t="s">
+      <c r="D50" s="308" t="s">
         <v>13</v>
       </c>
-      <c r="E50" s="313"/>
+      <c r="E50" s="308"/>
       <c r="F50" s="120">
         <f>F47-K49-C47</f>
         <v>1824260.97</v>
@@ -19596,22 +19761,22 @@
       <c r="Q50" s="9"/>
     </row>
     <row r="51" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D51" s="314" t="s">
+      <c r="D51" s="309" t="s">
         <v>14</v>
       </c>
-      <c r="E51" s="314"/>
+      <c r="E51" s="309"/>
       <c r="F51" s="115">
         <v>-1848136.64</v>
       </c>
-      <c r="I51" s="315" t="s">
+      <c r="I51" s="310" t="s">
         <v>15</v>
       </c>
-      <c r="J51" s="316"/>
-      <c r="K51" s="317">
+      <c r="J51" s="311"/>
+      <c r="K51" s="312">
         <f>F53+F54+F55</f>
         <v>195541.70000000007</v>
       </c>
-      <c r="L51" s="318"/>
+      <c r="L51" s="313"/>
       <c r="P51" s="34"/>
       <c r="Q51" s="9"/>
     </row>
@@ -19642,11 +19807,11 @@
         <v>17</v>
       </c>
       <c r="J53" s="130"/>
-      <c r="K53" s="319">
+      <c r="K53" s="314">
         <f>-C4</f>
         <v>-184342.19</v>
       </c>
-      <c r="L53" s="320"/>
+      <c r="L53" s="315"/>
     </row>
     <row r="54" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D54" s="131" t="s">
@@ -19663,22 +19828,22 @@
       <c r="C55" s="133">
         <v>44647</v>
       </c>
-      <c r="D55" s="296" t="s">
+      <c r="D55" s="291" t="s">
         <v>20</v>
       </c>
-      <c r="E55" s="297"/>
+      <c r="E55" s="292"/>
       <c r="F55" s="134">
         <v>219417.37</v>
       </c>
-      <c r="I55" s="298" t="s">
+      <c r="I55" s="293" t="s">
         <v>226</v>
       </c>
-      <c r="J55" s="299"/>
-      <c r="K55" s="300">
+      <c r="J55" s="294"/>
+      <c r="K55" s="295">
         <f>K51+K53</f>
         <v>11199.510000000068</v>
       </c>
-      <c r="L55" s="300"/>
+      <c r="L55" s="295"/>
     </row>
     <row r="56" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C56" s="135"/>
@@ -21320,23 +21485,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="283"/>
-      <c r="C1" s="285" t="s">
+      <c r="B1" s="278"/>
+      <c r="C1" s="280" t="s">
         <v>225</v>
       </c>
-      <c r="D1" s="286"/>
-      <c r="E1" s="286"/>
-      <c r="F1" s="286"/>
-      <c r="G1" s="286"/>
-      <c r="H1" s="286"/>
-      <c r="I1" s="286"/>
-      <c r="J1" s="286"/>
-      <c r="K1" s="286"/>
-      <c r="L1" s="286"/>
-      <c r="M1" s="286"/>
+      <c r="D1" s="281"/>
+      <c r="E1" s="281"/>
+      <c r="F1" s="281"/>
+      <c r="G1" s="281"/>
+      <c r="H1" s="281"/>
+      <c r="I1" s="281"/>
+      <c r="J1" s="281"/>
+      <c r="K1" s="281"/>
+      <c r="L1" s="281"/>
+      <c r="M1" s="281"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="284"/>
+      <c r="B2" s="279"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -21346,21 +21511,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="287" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="288"/>
+      <c r="B3" s="282" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="283"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="289" t="s">
+      <c r="H3" s="284" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="289"/>
+      <c r="I3" s="284"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="R3" s="294" t="s">
+      <c r="R3" s="289" t="s">
         <v>38</v>
       </c>
     </row>
@@ -21375,14 +21540,14 @@
       <c r="D4" s="18">
         <v>44647</v>
       </c>
-      <c r="E4" s="290" t="s">
+      <c r="E4" s="285" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="291"/>
-      <c r="H4" s="292" t="s">
+      <c r="F4" s="286"/>
+      <c r="H4" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="293"/>
+      <c r="I4" s="288"/>
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
       <c r="L4" s="21"/>
@@ -21392,11 +21557,11 @@
       <c r="N4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="301" t="s">
+      <c r="P4" s="296" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="302"/>
-      <c r="R4" s="295"/>
+      <c r="Q4" s="297"/>
+      <c r="R4" s="290"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
@@ -23040,11 +23205,11 @@
         <f>927.48+128</f>
         <v>1055.48</v>
       </c>
-      <c r="M40" s="303">
+      <c r="M40" s="298">
         <f>SUM(M5:M39)</f>
         <v>2146671</v>
       </c>
-      <c r="N40" s="305">
+      <c r="N40" s="300">
         <f>SUM(N5:N39)</f>
         <v>68590</v>
       </c>
@@ -23076,8 +23241,8 @@
       <c r="L41" s="75">
         <v>1195.68</v>
       </c>
-      <c r="M41" s="304"/>
-      <c r="N41" s="306"/>
+      <c r="M41" s="299"/>
+      <c r="N41" s="301"/>
       <c r="P41" s="34"/>
       <c r="Q41" s="9"/>
     </row>
@@ -23312,29 +23477,29 @@
       <c r="A53" s="117"/>
       <c r="B53" s="118"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="307" t="s">
+      <c r="H53" s="302" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="308"/>
+      <c r="I53" s="303"/>
       <c r="J53" s="119"/>
-      <c r="K53" s="309">
+      <c r="K53" s="304">
         <f>I51+L51</f>
         <v>91272.77</v>
       </c>
-      <c r="L53" s="310"/>
-      <c r="M53" s="311">
+      <c r="L53" s="305"/>
+      <c r="M53" s="306">
         <f>N40+M40</f>
         <v>2215261</v>
       </c>
-      <c r="N53" s="312"/>
+      <c r="N53" s="307"/>
       <c r="P53" s="34"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="313" t="s">
+      <c r="D54" s="308" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="313"/>
+      <c r="E54" s="308"/>
       <c r="F54" s="120">
         <f>F51-K53-C51</f>
         <v>2179879.23</v>
@@ -23345,22 +23510,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="314" t="s">
+      <c r="D55" s="309" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="314"/>
+      <c r="E55" s="309"/>
       <c r="F55" s="115">
         <v>-2227493.48</v>
       </c>
-      <c r="I55" s="315" t="s">
+      <c r="I55" s="310" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="316"/>
-      <c r="K55" s="317">
+      <c r="J55" s="311"/>
+      <c r="K55" s="312">
         <f>F57+F58+F59</f>
         <v>261521.34000000003</v>
       </c>
-      <c r="L55" s="318"/>
+      <c r="L55" s="313"/>
       <c r="P55" s="34"/>
       <c r="Q55" s="9"/>
     </row>
@@ -23391,11 +23556,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="130"/>
-      <c r="K57" s="319">
+      <c r="K57" s="314">
         <f>-C4</f>
         <v>-219417.37</v>
       </c>
-      <c r="L57" s="320"/>
+      <c r="L57" s="315"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="131" t="s">
@@ -23412,22 +23577,22 @@
       <c r="C59" s="133">
         <v>44682</v>
       </c>
-      <c r="D59" s="296" t="s">
+      <c r="D59" s="291" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="297"/>
+      <c r="E59" s="292"/>
       <c r="F59" s="134">
         <v>297874.59000000003</v>
       </c>
-      <c r="I59" s="298" t="s">
+      <c r="I59" s="293" t="s">
         <v>168</v>
       </c>
-      <c r="J59" s="299"/>
-      <c r="K59" s="300">
+      <c r="J59" s="294"/>
+      <c r="K59" s="295">
         <f>K55+K57</f>
         <v>42103.97000000003</v>
       </c>
-      <c r="L59" s="300"/>
+      <c r="L59" s="295"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="135"/>
@@ -25050,10 +25215,10 @@
   <dimension ref="A1:U81"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="F23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25076,23 +25241,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="283"/>
-      <c r="C1" s="285" t="s">
+      <c r="B1" s="278"/>
+      <c r="C1" s="280" t="s">
         <v>277</v>
       </c>
-      <c r="D1" s="286"/>
-      <c r="E1" s="286"/>
-      <c r="F1" s="286"/>
-      <c r="G1" s="286"/>
-      <c r="H1" s="286"/>
-      <c r="I1" s="286"/>
-      <c r="J1" s="286"/>
-      <c r="K1" s="286"/>
-      <c r="L1" s="286"/>
-      <c r="M1" s="286"/>
+      <c r="D1" s="281"/>
+      <c r="E1" s="281"/>
+      <c r="F1" s="281"/>
+      <c r="G1" s="281"/>
+      <c r="H1" s="281"/>
+      <c r="I1" s="281"/>
+      <c r="J1" s="281"/>
+      <c r="K1" s="281"/>
+      <c r="L1" s="281"/>
+      <c r="M1" s="281"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="284"/>
+      <c r="B2" s="279"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -25102,21 +25267,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="287" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="288"/>
+      <c r="B3" s="282" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="283"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="289" t="s">
+      <c r="H3" s="284" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="289"/>
+      <c r="I3" s="284"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="R3" s="294" t="s">
+      <c r="R3" s="289" t="s">
         <v>38</v>
       </c>
     </row>
@@ -25131,14 +25296,14 @@
       <c r="D4" s="18">
         <v>44682</v>
       </c>
-      <c r="E4" s="290" t="s">
+      <c r="E4" s="285" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="291"/>
-      <c r="H4" s="292" t="s">
+      <c r="F4" s="286"/>
+      <c r="H4" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="293"/>
+      <c r="I4" s="288"/>
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
       <c r="L4" s="21"/>
@@ -25148,11 +25313,11 @@
       <c r="N4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="301" t="s">
+      <c r="P4" s="296" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="302"/>
-      <c r="R4" s="295"/>
+      <c r="Q4" s="297"/>
+      <c r="R4" s="290"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
@@ -26207,7 +26372,7 @@
       <c r="B27" s="25">
         <v>44705</v>
       </c>
-      <c r="C27" s="274">
+      <c r="C27" s="26">
         <v>2800</v>
       </c>
       <c r="D27" s="41" t="s">
@@ -26216,14 +26381,14 @@
       <c r="E27" s="28">
         <v>44705</v>
       </c>
-      <c r="F27" s="272">
+      <c r="F27" s="29">
         <v>68453</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="30">
         <v>44705</v>
       </c>
-      <c r="I27" s="273">
+      <c r="I27" s="31">
         <v>43</v>
       </c>
       <c r="J27" s="67"/>
@@ -26254,21 +26419,21 @@
       <c r="B28" s="25">
         <v>44706</v>
       </c>
-      <c r="C28" s="274">
+      <c r="C28" s="26">
         <v>0</v>
       </c>
       <c r="D28" s="41"/>
       <c r="E28" s="28">
         <v>44706</v>
       </c>
-      <c r="F28" s="272">
+      <c r="F28" s="29">
         <v>28820</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="30">
         <v>44706</v>
       </c>
-      <c r="I28" s="273">
+      <c r="I28" s="31">
         <v>1153</v>
       </c>
       <c r="J28" s="69"/>
@@ -26278,16 +26443,15 @@
         <f>16978+10000</f>
         <v>26978</v>
       </c>
-      <c r="N28" s="276">
+      <c r="N28" s="33">
         <v>689</v>
       </c>
       <c r="P28" s="34">
         <f t="shared" si="0"/>
         <v>28820</v>
       </c>
-      <c r="Q28" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="Q28" s="13" t="s">
+        <v>8</v>
       </c>
       <c r="R28" s="8"/>
       <c r="S28">
@@ -26299,7 +26463,7 @@
       <c r="B29" s="25">
         <v>44707</v>
       </c>
-      <c r="C29" s="274">
+      <c r="C29" s="26">
         <v>20289</v>
       </c>
       <c r="D29" s="71" t="s">
@@ -26308,24 +26472,24 @@
       <c r="E29" s="28">
         <v>44707</v>
       </c>
-      <c r="F29" s="272">
+      <c r="F29" s="29">
         <v>65956</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="30">
         <v>44707</v>
       </c>
-      <c r="I29" s="273">
+      <c r="I29" s="31">
         <v>93</v>
       </c>
       <c r="J29" s="67"/>
       <c r="K29" s="72"/>
       <c r="L29" s="66"/>
-      <c r="M29" s="275">
+      <c r="M29" s="32">
         <f>20000+25531</f>
         <v>45531</v>
       </c>
-      <c r="N29" s="276">
+      <c r="N29" s="33">
         <v>43</v>
       </c>
       <c r="P29" s="34">
@@ -26684,7 +26848,7 @@
       <c r="J39" s="73">
         <v>44710</v>
       </c>
-      <c r="K39" s="282" t="s">
+      <c r="K39" s="277" t="s">
         <v>320</v>
       </c>
       <c r="L39" s="75">
@@ -26717,11 +26881,11 @@
       <c r="J40" s="73"/>
       <c r="K40" s="76"/>
       <c r="L40" s="75"/>
-      <c r="M40" s="303">
+      <c r="M40" s="298">
         <f>SUM(M5:M39)</f>
         <v>2144215</v>
       </c>
-      <c r="N40" s="305">
+      <c r="N40" s="300">
         <f>SUM(N5:N39)</f>
         <v>62525</v>
       </c>
@@ -26747,8 +26911,8 @@
       <c r="J41" s="73"/>
       <c r="K41" s="245"/>
       <c r="L41" s="75"/>
-      <c r="M41" s="304"/>
-      <c r="N41" s="306"/>
+      <c r="M41" s="299"/>
+      <c r="N41" s="301"/>
       <c r="P41" s="34"/>
       <c r="Q41" s="9"/>
     </row>
@@ -26963,29 +27127,29 @@
       <c r="A53" s="117"/>
       <c r="B53" s="118"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="307" t="s">
+      <c r="H53" s="302" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="308"/>
+      <c r="I53" s="303"/>
       <c r="J53" s="119"/>
-      <c r="K53" s="309">
+      <c r="K53" s="304">
         <f>I51+L51</f>
         <v>51231.42</v>
       </c>
-      <c r="L53" s="310"/>
-      <c r="M53" s="311">
+      <c r="L53" s="305"/>
+      <c r="M53" s="306">
         <f>N40+M40</f>
         <v>2206740</v>
       </c>
-      <c r="N53" s="312"/>
+      <c r="N53" s="307"/>
       <c r="P53" s="34"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="313" t="s">
+      <c r="D54" s="308" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="313"/>
+      <c r="E54" s="308"/>
       <c r="F54" s="120">
         <f>F51-K53-C51</f>
         <v>2189405.58</v>
@@ -26996,22 +27160,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="314" t="s">
+      <c r="D55" s="309" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="314"/>
+      <c r="E55" s="309"/>
       <c r="F55" s="115">
         <v>-2251924.65</v>
       </c>
-      <c r="I55" s="315" t="s">
+      <c r="I55" s="310" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="316"/>
-      <c r="K55" s="317">
+      <c r="J55" s="311"/>
+      <c r="K55" s="312">
         <f>F57+F58+F59</f>
         <v>112552.74000000017</v>
       </c>
-      <c r="L55" s="318"/>
+      <c r="L55" s="313"/>
       <c r="P55" s="34"/>
       <c r="Q55" s="9"/>
     </row>
@@ -27042,11 +27206,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="130"/>
-      <c r="K57" s="319">
+      <c r="K57" s="314">
         <f>-C4</f>
         <v>-297874.59000000003</v>
       </c>
-      <c r="L57" s="320"/>
+      <c r="L57" s="315"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="131" t="s">
@@ -27063,22 +27227,22 @@
       <c r="C59" s="133">
         <v>44710</v>
       </c>
-      <c r="D59" s="296" t="s">
+      <c r="D59" s="291" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="297"/>
+      <c r="E59" s="292"/>
       <c r="F59" s="134">
         <v>149938.81</v>
       </c>
-      <c r="I59" s="298" t="s">
+      <c r="I59" s="293" t="s">
         <v>325</v>
       </c>
-      <c r="J59" s="299"/>
-      <c r="K59" s="300">
+      <c r="J59" s="294"/>
+      <c r="K59" s="295">
         <f>K55+K57</f>
         <v>-185321.84999999986</v>
       </c>
-      <c r="L59" s="300"/>
+      <c r="L59" s="295"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="135"/>

</xml_diff>